<commit_message>
First draft of complete QB creation process; elaborated on the formulae used to adjust salaries and bonus for deflation; further alterations to the Latest Player Attributes.csv file and BAKs of it; removed superfluous BAKs in the output folder; altered Methods for Setting Field Values.xlsx to reflect final decisions on process for QBs.
</commit_message>
<xml_diff>
--- a/docs/2017_12 Debugging/Contracts Comparison 2018_01_09.xlsx
+++ b/docs/2017_12 Debugging/Contracts Comparison 2018_01_09.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>Per Year Min:</t>
   </si>
@@ -65,33 +65,92 @@
     <t>Proposed Rules:</t>
   </si>
   <si>
-    <t>Total Sal &lt; 1M, cut to 50%</t>
-  </si>
-  <si>
-    <t>Total Sal &gt; 10M, cut to 75%</t>
-  </si>
-  <si>
-    <t>Signing Bon &lt; 100K, cut to 75%</t>
-  </si>
-  <si>
-    <t>Signing Bon &gt;100K, &lt; 1M, cut to 60%</t>
-  </si>
-  <si>
     <t>Signing Bon &gt;1M, &lt; 10M, cut to 50%</t>
   </si>
   <si>
     <t>Signing Bon &gt;10M, cut to 40%</t>
   </si>
   <si>
-    <t>Total Sal &gt; 1M, &lt; 10M, cut to 60%</t>
+    <t>Total Sal &lt; 1M, cut to 43%</t>
+  </si>
+  <si>
+    <t>Total Sal &gt; 10M, cut to 72.5%</t>
+  </si>
+  <si>
+    <t>NOTE!! PSBO must always be in multiples of PCON (length of contract). This means if the contract is for 3 years, the bonus can NOT be 10,000 or 20,000 (PSBO != 1 or 2).</t>
+  </si>
+  <si>
+    <t>Total Sal &gt; 1M, &lt; 10M, cut to 58%</t>
+  </si>
+  <si>
+    <t>Formula:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if tot_sal &gt; 10M: </t>
+  </si>
+  <si>
+    <t>new_tot_sal = round((tot_sal / 10000) * .725)</t>
+  </si>
+  <si>
+    <t>elif tot_sal &gt; 1M:</t>
+  </si>
+  <si>
+    <t>new_tot_sal = round((tot_sal / 10000) * .58)</t>
+  </si>
+  <si>
+    <t>new_tot_sal = round((tot_sal / 10000) * .43)</t>
+  </si>
+  <si>
+    <t>else:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if sgn_bon &gt; 10M: </t>
+  </si>
+  <si>
+    <t>Signing Bon &lt; 100K, cut to 80%</t>
+  </si>
+  <si>
+    <t>Signing Bon &gt;100K, &lt; 1M, cut to 65%</t>
+  </si>
+  <si>
+    <t>new_sgn_bon = round((sgn_bon / 10000) * .4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elif sgn_bon &gt; 1M: </t>
+  </si>
+  <si>
+    <t>new_sgn_bon = round((sgn_bon / 10000) * .5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elif sgn_bon &gt; 100K: </t>
+  </si>
+  <si>
+    <t>new_sgn_bon = round((sgn_bon / 10000) * .65)</t>
+  </si>
+  <si>
+    <t>new_sgn_bon = round((sgn_bon / 10000) * .8)</t>
+  </si>
+  <si>
+    <t>AND then:</t>
+  </si>
+  <si>
+    <t>if (new_sgn_bon Mod PCON) &gt; 0: new_sgn_bon +=  PCON - (new_sgn_bon Mod PCON)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -121,8 +180,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,27 +464,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="4" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -431,10 +493,10 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>200000</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>465000</v>
       </c>
       <c r="D2">
@@ -446,147 +508,235 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>14171500</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>23943600</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D9" si="0">(B3/C3)*100</f>
+        <f t="shared" ref="D3:D12" si="0">(B3/C3)*100</f>
         <v>59.187006131074696</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B5" s="1">
         <v>10000</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C5" s="1">
         <v>41000</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <f t="shared" si="0"/>
         <v>24.390243902439025</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B6" s="1">
         <v>10811500</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C6" s="1">
         <v>14170833</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <f t="shared" si="0"/>
         <v>76.294032961929616</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B8" s="1">
         <v>230000</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C8" s="1">
         <v>465000</v>
       </c>
-      <c r="D6">
+      <c r="D8">
         <f t="shared" si="0"/>
         <v>49.462365591397848</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B9" s="1">
         <v>99200000</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C9" s="1">
         <v>135000000</v>
       </c>
-      <c r="D7">
+      <c r="D9">
         <f t="shared" si="0"/>
         <v>73.481481481481481</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B11" s="1">
         <v>0</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C11" s="1">
         <v>0</v>
       </c>
-      <c r="D8">
+      <c r="D11">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B12" s="1">
         <v>23520000</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C12" s="1">
         <v>60500000</v>
       </c>
-      <c r="D9">
+      <c r="D12">
         <f t="shared" si="0"/>
         <v>38.876033057851238</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-    </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>18</v>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>